<commit_message>
refactor customer import attention
</commit_message>
<xml_diff>
--- a/storage/app/import/customer.xlsx
+++ b/storage/app/import/customer.xlsx
@@ -598,7 +598,7 @@
     <t xml:space="preserve">PT. Sayap Garuda Indah</t>
   </si>
   <si>
-    <t xml:space="preserve">Dewa Ruci Building No. 2, By Pass Ngurah Ray, Simp</t>
+    <t xml:space="preserve">Dewa Ruci Building No. 2 Jalan ByPass Ngurah Rai Simpang Siur, Kuta 80361 Bali</t>
   </si>
   <si>
     <t xml:space="preserve">0361-767466</t>
@@ -673,7 +673,7 @@
     <t xml:space="preserve">Transwisata Prima Aviation</t>
   </si>
   <si>
-    <t xml:space="preserve">Halim Perdana Kusuma Airport Lt.2 rOOM 225</t>
+    <t xml:space="preserve">Halim Perdana Kusuma Airport Lt.2 Room 225</t>
   </si>
   <si>
     <t xml:space="preserve">021-80889628, 808995</t>
@@ -691,7 +691,7 @@
     <t xml:space="preserve">Wings Air</t>
   </si>
   <si>
-    <t xml:space="preserve">Kawasn Kasatlan Angkatan Laut, Jl. Raya Juana</t>
+    <t xml:space="preserve">Kawasan Kasatlan Angkatan Laut, Jl. Raya Juana</t>
   </si>
   <si>
     <t xml:space="preserve">021-63860180;0877-0315-4325;0899-1848-399</t>
@@ -1329,8 +1329,8 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35:B46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2598,7 +2598,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>191</v>
       </c>
@@ -2770,7 +2770,7 @@
       <c r="R33" s="2"/>
       <c r="S33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
         <v>216</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="R34" s="2"/>
       <c r="S34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26" t="s">
         <v>222</v>
       </c>

</xml_diff>